<commit_message>
Stats pour 16 noeuds
</commit_message>
<xml_diff>
--- a/M2/Parallelisme/Optimisation/TP3/Perf-MatrixProd-MPI.xlsx
+++ b/M2/Parallelisme/Optimisation/TP3/Perf-MatrixProd-MPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspaces\Cours\M2\Parallelisme\Optimisation\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB2462B-90AE-4021-9E84-FF03E3A84A8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8B4E23-5790-4B10-A101-A6259DF7AC34}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>FUCHS</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>8192x8192</t>
-  </si>
-  <si>
-    <t>16 processeurs de 4 cœurs physiques hyperthreadés</t>
   </si>
   <si>
     <r>
@@ -427,6 +424,27 @@
       </rPr>
       <t>kernel 1</t>
     </r>
+  </si>
+  <si>
+    <t>mpirun -np 64 -map-by ppr:1:socket -rank-by socket -bind-to socket -machinefile machines.txt ./MatrixProduct -klc 8 -k 1 -nt 1</t>
+  </si>
+  <si>
+    <t>mpirun -np 256 -map-by ppr:1:core -rank-by core -bind-to core -machinefile machines.txt ./MatrixProduct -klc 8 -k 1 -nt 1</t>
+  </si>
+  <si>
+    <t>mpirun -np 256 -map-by ppr:1:core -rank-by node -bind-to core -machinefile machines.txt ./MatrixProduct -klc 8 -k 1 -nt 1</t>
+  </si>
+  <si>
+    <t>32 PC avec 2 processeurs de 4 cœurs physiques hyperthreadés</t>
+  </si>
+  <si>
+    <t>np = 2 socket * Nmachines</t>
+  </si>
+  <si>
+    <t>np = 4 coeurs * Nmachines</t>
+  </si>
+  <si>
+    <t>mpirun -np 64 -map-by ppr:1:socket -rank-by socket -bind-to socket -machinefile machines.txt ./MatrixProduct -klc 8 -k 1 -nt 4</t>
   </si>
 </sst>
 </file>
@@ -964,13 +982,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36:G37"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="105" customWidth="1"/>
     <col min="2" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="1025" width="9.140625" customWidth="1"/>
   </cols>
@@ -1024,13 +1042,21 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1041,7 +1067,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="9">
         <v>1</v>
@@ -1064,103 +1090,115 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="11">
-        <v>26.61</v>
+        <v>13.69</v>
       </c>
       <c r="C12" s="11">
-        <v>13.69</v>
+        <v>6.95</v>
       </c>
       <c r="D12" s="11">
-        <v>6.95</v>
+        <v>3.88</v>
       </c>
       <c r="E12" s="11">
-        <v>3.88</v>
-      </c>
-      <c r="F12" s="11"/>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1.69</v>
+      </c>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="11">
-        <v>41.311</v>
+        <v>80.3</v>
       </c>
       <c r="C13" s="11">
-        <v>80.3</v>
+        <v>158.05000000000001</v>
       </c>
       <c r="D13" s="11">
-        <v>158.05000000000001</v>
+        <v>282.98</v>
       </c>
       <c r="E13" s="11">
-        <v>282.98</v>
-      </c>
-      <c r="F13" s="11"/>
+        <v>44.32</v>
+      </c>
+      <c r="F13" s="11">
+        <v>647.13</v>
+      </c>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11">
+        <f>B13/$B$13</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <f>C13/$B$13</f>
+        <v>1.9682440846824412</v>
+      </c>
+      <c r="D14" s="11">
+        <f>D13/$B$13</f>
+        <v>3.5240348692403489</v>
+      </c>
+      <c r="E14" s="11">
+        <f>E13/$B$13</f>
+        <v>0.55193026151930269</v>
+      </c>
+      <c r="F14" s="11">
+        <f>F13/$B$13</f>
+        <v>8.0589041095890419</v>
+      </c>
+      <c r="G14" s="11">
+        <f>G13/$B$13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
-        <f t="shared" ref="B14:G14" si="0">B13/$B$13</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="11">
+      <c r="B15" s="12">
+        <f t="shared" ref="B15:G15" si="0">B14/B11*100</f>
+        <v>100</v>
+      </c>
+      <c r="C15" s="12">
         <f t="shared" si="0"/>
-        <v>1.9437922103071821</v>
-      </c>
-      <c r="D14" s="11">
+        <v>98.412204234122058</v>
+      </c>
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
-        <v>3.8258575197889186</v>
-      </c>
-      <c r="E14" s="11">
+        <v>88.100871731008723</v>
+      </c>
+      <c r="E15" s="12">
         <f t="shared" si="0"/>
-        <v>6.8499915276802792</v>
-      </c>
-      <c r="F14" s="11">
+        <v>6.8991282689912836</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>50.368150684931514</v>
+      </c>
+      <c r="G15" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="12">
-        <f t="shared" ref="B15:G15" si="1">B14/B11*100</f>
-        <v>100</v>
-      </c>
-      <c r="C15" s="12">
-        <f t="shared" si="1"/>
-        <v>97.189610515359107</v>
-      </c>
-      <c r="D15" s="12">
-        <f t="shared" si="1"/>
-        <v>95.646437994722959</v>
-      </c>
-      <c r="E15" s="12">
-        <f t="shared" si="1"/>
-        <v>85.624894096003487</v>
-      </c>
-      <c r="F15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1171,7 +1209,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
@@ -1194,103 +1232,115 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="11">
-        <v>7.34</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="C20" s="11">
-        <v>4.1399999999999997</v>
+        <v>2.44</v>
       </c>
       <c r="D20" s="11">
-        <v>2.44</v>
+        <v>1.74</v>
       </c>
       <c r="E20" s="11">
-        <v>1.74</v>
-      </c>
-      <c r="F20" s="11"/>
+        <v>1.24</v>
+      </c>
+      <c r="F20" s="11">
+        <v>1.06</v>
+      </c>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="11">
-        <v>149.59</v>
+        <v>265.02</v>
       </c>
       <c r="C21" s="11">
-        <v>265.02</v>
+        <v>448.85</v>
       </c>
       <c r="D21" s="11">
-        <v>448.85</v>
+        <v>631.71</v>
       </c>
       <c r="E21" s="11">
-        <v>631.71</v>
-      </c>
-      <c r="F21" s="11"/>
+        <v>884.44</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1034.17</v>
+      </c>
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" ref="B22:G22" si="1">B21/$B$21</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="1"/>
+        <v>1.693645762583956</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="1"/>
+        <v>2.3836314240434686</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="1"/>
+        <v>3.3372575654667576</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="1"/>
+        <v>3.9022337936759497</v>
+      </c>
+      <c r="G22" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="11">
-        <f t="shared" ref="B22:G22" si="2">B21/$B$21</f>
-        <v>1</v>
-      </c>
-      <c r="C22" s="11">
+      <c r="B23" s="12">
+        <f t="shared" ref="B23:G23" si="2">B22/B19*100</f>
+        <v>100</v>
+      </c>
+      <c r="C23" s="12">
         <f t="shared" si="2"/>
-        <v>1.7716424894712213</v>
-      </c>
-      <c r="D22" s="11">
+        <v>84.682288129197801</v>
+      </c>
+      <c r="D23" s="12">
         <f t="shared" si="2"/>
-        <v>3.000534795106625</v>
-      </c>
-      <c r="E22" s="11">
+        <v>59.590785601086715</v>
+      </c>
+      <c r="E23" s="12">
         <f t="shared" si="2"/>
-        <v>4.2229427100742027</v>
-      </c>
-      <c r="F22" s="11">
+        <v>41.715719568334471</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="2"/>
+        <v>24.388961210474687</v>
+      </c>
+      <c r="G23" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G22" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="12">
-        <f t="shared" ref="B23:G23" si="3">B22/B19*100</f>
-        <v>100</v>
-      </c>
-      <c r="C23" s="12">
-        <f t="shared" si="3"/>
-        <v>88.582124473561066</v>
-      </c>
-      <c r="D23" s="12">
-        <f t="shared" si="3"/>
-        <v>75.013369877665625</v>
-      </c>
-      <c r="E23" s="12">
-        <f t="shared" si="3"/>
-        <v>52.786783875927533</v>
-      </c>
-      <c r="F23" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1301,7 +1351,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
@@ -1324,103 +1374,115 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="11">
-        <v>26.62</v>
+        <v>6.87</v>
       </c>
       <c r="C28" s="11">
-        <v>13.26</v>
+        <v>3.99</v>
       </c>
       <c r="D28" s="11">
-        <v>6.87</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="E28" s="11">
-        <v>3.99</v>
-      </c>
-      <c r="F28" s="11"/>
+        <v>1.52</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1.21</v>
+      </c>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29" s="11">
-        <v>41.3</v>
+        <v>160.01</v>
       </c>
       <c r="C29" s="11">
-        <v>82.91</v>
+        <v>275.49</v>
       </c>
       <c r="D29" s="11">
-        <v>160.01</v>
+        <v>444.09</v>
       </c>
       <c r="E29" s="11">
-        <v>275.49</v>
-      </c>
-      <c r="F29" s="11"/>
+        <v>721.41</v>
+      </c>
+      <c r="F29" s="11">
+        <v>906.59</v>
+      </c>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="11">
+        <f t="shared" ref="B30:G30" si="3">B29/$B$29</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="11">
+        <f t="shared" si="3"/>
+        <v>1.7217048934441599</v>
+      </c>
+      <c r="D30" s="11">
+        <f t="shared" si="3"/>
+        <v>2.7753890381851134</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" si="3"/>
+        <v>4.5085307168301982</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="3"/>
+        <v>5.6658333854134124</v>
+      </c>
+      <c r="G30" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="11">
-        <f t="shared" ref="B30:G30" si="4">B29/$B$29</f>
-        <v>1</v>
-      </c>
-      <c r="C30" s="11">
+      <c r="B31" s="12">
+        <f t="shared" ref="B31:G31" si="4">B30/B27*100</f>
+        <v>100</v>
+      </c>
+      <c r="C31" s="12">
         <f t="shared" si="4"/>
-        <v>2.0075060532687652</v>
-      </c>
-      <c r="D30" s="11">
+        <v>86.085244672207992</v>
+      </c>
+      <c r="D31" s="12">
         <f t="shared" si="4"/>
-        <v>3.8743341404358356</v>
-      </c>
-      <c r="E30" s="11">
+        <v>69.384725954627839</v>
+      </c>
+      <c r="E31" s="12">
         <f t="shared" si="4"/>
-        <v>6.6704600484261505</v>
-      </c>
-      <c r="F30" s="11">
+        <v>56.356633960377479</v>
+      </c>
+      <c r="F31" s="12">
+        <f t="shared" si="4"/>
+        <v>35.41145865883383</v>
+      </c>
+      <c r="G31" s="12">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G30" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="12">
-        <f t="shared" ref="B31:G31" si="5">B30/B27*100</f>
-        <v>100</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="5"/>
-        <v>100.37530266343826</v>
-      </c>
-      <c r="D31" s="12">
-        <f t="shared" si="5"/>
-        <v>96.858353510895896</v>
-      </c>
-      <c r="E31" s="12">
-        <f t="shared" si="5"/>
-        <v>83.380750605326881</v>
-      </c>
-      <c r="F31" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="12">
-        <f t="shared" si="5"/>
-        <v>0</v>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1431,7 +1493,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="8">
         <v>1</v>
@@ -1454,97 +1516,101 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="11">
-        <v>26.39</v>
+        <v>6.87</v>
       </c>
       <c r="C36" s="11">
-        <v>13.92</v>
+        <v>3.9</v>
       </c>
       <c r="D36" s="11">
-        <v>7.53</v>
+        <v>6.22</v>
       </c>
       <c r="E36" s="11">
-        <v>4.63</v>
-      </c>
-      <c r="F36" s="11"/>
+        <v>5.16</v>
+      </c>
+      <c r="F36" s="11">
+        <v>5.03</v>
+      </c>
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="11">
-        <v>41.64</v>
+        <v>159.97</v>
       </c>
       <c r="C37" s="11">
-        <v>78.97</v>
+        <v>281.56</v>
       </c>
       <c r="D37" s="11">
-        <v>145.93</v>
+        <v>176.62</v>
       </c>
       <c r="E37" s="11">
-        <v>237.19</v>
-      </c>
-      <c r="F37" s="11"/>
+        <v>212.95</v>
+      </c>
+      <c r="F37" s="11">
+        <v>218.35</v>
+      </c>
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="11">
-        <f t="shared" ref="B38:G38" si="6">B37/$B$37</f>
+        <f t="shared" ref="B38:G38" si="5">B37/$B$37</f>
         <v>1</v>
       </c>
       <c r="C38" s="11">
-        <f t="shared" si="6"/>
-        <v>1.8964937560038424</v>
+        <f t="shared" si="5"/>
+        <v>1.7600800150028131</v>
       </c>
       <c r="D38" s="11">
-        <f t="shared" si="6"/>
-        <v>3.5045629202689721</v>
+        <f t="shared" si="5"/>
+        <v>1.1040820153778834</v>
       </c>
       <c r="E38" s="11">
-        <f t="shared" si="6"/>
-        <v>5.6962055715658018</v>
+        <f t="shared" si="5"/>
+        <v>1.3311870975807962</v>
       </c>
       <c r="F38" s="11">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1.3649434268925422</v>
       </c>
       <c r="G38" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B39" s="12">
-        <f t="shared" ref="B39:G39" si="7">B38/B35*100</f>
+        <f t="shared" ref="B39:G39" si="6">B38/B35*100</f>
         <v>100</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" si="7"/>
-        <v>94.824687800192123</v>
+        <f t="shared" si="6"/>
+        <v>88.004000750140648</v>
       </c>
       <c r="D39" s="12">
-        <f t="shared" si="7"/>
-        <v>87.614073006724297</v>
+        <f t="shared" si="6"/>
+        <v>27.602050384447086</v>
       </c>
       <c r="E39" s="12">
-        <f t="shared" si="7"/>
-        <v>71.20256964457252</v>
+        <f t="shared" si="6"/>
+        <v>16.639838719759954</v>
       </c>
       <c r="F39" s="12">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>8.5308964180783882</v>
       </c>
       <c r="G39" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1556,6 +1622,6 @@
     <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>